<commit_message>
Adding Admin Test cases
</commit_message>
<xml_diff>
--- a/Config/Test_Data_List.xlsx
+++ b/Config/Test_Data_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firdi/Downloads/Products-master/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F8EB26-ACC3-1A41-9AF7-524DD1FEF350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCED2639-4E79-B048-9086-717EBD3A699B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="1" xr2:uid="{E7AFE29E-E74F-8642-80B4-6E9C778320BD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>test_Login</t>
   </si>
@@ -185,6 +185,51 @@
   </si>
   <si>
     <t>Dashboard All Quiz Category Batch Quiz</t>
+  </si>
+  <si>
+    <t>AddQuestion</t>
+  </si>
+  <si>
+    <t>option1</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>option3</t>
+  </si>
+  <si>
+    <t>option4</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+  <si>
+    <t>what are variables</t>
+  </si>
+  <si>
+    <t>Var are functions</t>
+  </si>
+  <si>
+    <t>Var are classes</t>
+  </si>
+  <si>
+    <t>Var are unnamed memory location</t>
+  </si>
+  <si>
+    <t>Var are constructors</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>option 3</t>
   </si>
 </sst>
 </file>
@@ -842,19 +887,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0445CD26-F25A-B54C-B67C-9475AA9C61F8}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="60.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
+    <col min="6" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -873,8 +920,29 @@
       <c r="F1" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -890,8 +958,36 @@
       <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>